<commit_message>
MechaBible Mark I: Programming - Python: Arduino GUI Multiple Windows, Database Connection, Data Analysis & Static Data Addition
</commit_message>
<xml_diff>
--- a/1.-Data Science/0.-Archivos_Ejercicios_Python/23.-GUI PyQt5 Conexion DataBase/23.-Reporte Analisis de Datos 1.xlsx
+++ b/1.-Data Science/0.-Archivos_Ejercicios_Python/23.-GUI PyQt5 Conexion DataBase/23.-Reporte Analisis de Datos 1.xlsx
@@ -1,20 +1,71 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\OneDrive\Documents\The_MechaBible\p_Python_ESP\1.-Data Science\0.-Archivos_Ejercicios_Python\23.-GUI PyQt5 Conexion DataBase\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A24A968D-B053-449D-ABEC-0FBCD74208BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="48">
+  <si>
+    <t>Title A1.1</t>
+  </si>
+  <si>
+    <t>Static Row 1</t>
+  </si>
+  <si>
+    <t>Static Row 2</t>
+  </si>
+  <si>
+    <t>Static Row 3</t>
+  </si>
+  <si>
+    <t>Static Row 4</t>
+  </si>
+  <si>
+    <t>Static Row 5</t>
+  </si>
+  <si>
+    <t>Static Row 6</t>
+  </si>
+  <si>
+    <t>Title A1.2</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>Title A1.3</t>
+  </si>
+  <si>
+    <t>Title A2</t>
+  </si>
+  <si>
+    <t>Subtitle A2.1</t>
+  </si>
+  <si>
+    <t>Subtitle A2.2</t>
+  </si>
+  <si>
+    <t>Subtitle A2.3</t>
+  </si>
+  <si>
+    <t>Static Text: Lorem ipsum dolor sit amet, consectetur adipiscing elit. Quisque non laoreet mauris. Pellentesque habitant morbi tristique senectus et netus et malesuada fames ac turpis egestas. Curabitur vulputate bibendum nibh elementum pulvinar. Integer a leo in orci ultricies fermentum. Ut vitae velit et sapien congue accumsan sed tincidunt dui. Ut elementum imperdiet nunc, non hendrerit enim ultrices at. Sed rhoncus vehicula.</t>
+  </si>
   <si>
     <t>Titulo Static</t>
   </si>
@@ -80,13 +131,46 @@
   </si>
   <si>
     <t>01-12-2023</t>
+  </si>
+  <si>
+    <t>Title B1</t>
+  </si>
+  <si>
+    <t>Title B1.1</t>
+  </si>
+  <si>
+    <t>Subtitle 1</t>
+  </si>
+  <si>
+    <t>Static Row 7</t>
+  </si>
+  <si>
+    <t>Subtitle 2</t>
+  </si>
+  <si>
+    <t>Title B1.2</t>
+  </si>
+  <si>
+    <t>Title B1.3</t>
+  </si>
+  <si>
+    <t>Title B1.4</t>
+  </si>
+  <si>
+    <t>Title B1.5</t>
+  </si>
+  <si>
+    <t>Title B1.6</t>
+  </si>
+  <si>
+    <t>Title B1.7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,16 +222,95 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="16">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD3DFEE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF808080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF808080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA7BFDE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF4F81BD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF4F81BD"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -158,33 +321,48 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD3D3D3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF4F81BD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF5EC268"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF008000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD3DFEE"/>
         </patternFill>
       </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -222,7 +400,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -256,6 +434,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -290,9 +469,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -465,161 +645,841 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:G16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="46.6640625" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E7" t="s">
+      <c r="B21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>21</v>
       </c>
+      <c r="B26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" t="s">
+        <v>44</v>
+      </c>
+      <c r="E30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" t="s">
+        <v>8</v>
+      </c>
+      <c r="F35" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" t="s">
+        <v>8</v>
+      </c>
+      <c r="F37" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" t="s">
+        <v>8</v>
+      </c>
+      <c r="F38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G38" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" t="s">
+        <v>8</v>
+      </c>
+      <c r="F39" t="s">
+        <v>8</v>
+      </c>
+      <c r="G39" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" t="s">
+        <v>8</v>
+      </c>
+      <c r="F40" t="s">
+        <v>8</v>
+      </c>
+      <c r="G40" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:E1">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+  <mergeCells count="13">
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="A29:G29"/>
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A11:G11"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="A13:G13"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A2:A8">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="2">
+      <formula>LEN(TRIM(A2))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A22:A28">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="17">
+      <formula>LEN(TRIM(A22))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32:A44">
+    <cfRule type="notContainsBlanks" dxfId="13" priority="25">
+      <formula>LEN(TRIM(A32))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:C1">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A7">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
-      <formula>LEN(TRIM(A2))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B7">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
+  <conditionalFormatting sqref="A21:E21">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="16">
+      <formula>LEN(TRIM(A21))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9:G9">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="5">
+      <formula>LEN(TRIM(A9))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10:G10">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="6">
+      <formula>LEN(TRIM(A10))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A29:G29">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="22">
+      <formula>LEN(TRIM(A29))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A30:G30">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="23">
+      <formula>LEN(TRIM(A30))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A31:G31">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="24">
+      <formula>LEN(TRIM(A31))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B8">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="3">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C7">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
+  <conditionalFormatting sqref="B22:B28">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="18">
+      <formula>LEN(TRIM(B22))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32:B44">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="26">
+      <formula>LEN(TRIM(B32))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C8">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="4">
       <formula>LEN(TRIM(C2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D7">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="5">
-      <formula>LEN(TRIM(D2))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E7">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="6">
-      <formula>LEN(TRIM(E2))&gt;0</formula>
+  <conditionalFormatting sqref="C22:E28">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="19">
+      <formula>LEN(TRIM(C22))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C32:G44">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="27">
+      <formula>LEN(TRIM(C32))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
MechaBible Mark I: Programming - Python: Arduino GUI Multiple Windows, Database Connection, Data Analysis, Static Data Addition & Excell Cell Auto Adjustment
</commit_message>
<xml_diff>
--- a/1.-Data Science/0.-Archivos_Ejercicios_Python/23.-GUI PyQt5 Conexion DataBase/23.-Reporte Analisis de Datos 1.xlsx
+++ b/1.-Data Science/0.-Archivos_Ejercicios_Python/23.-GUI PyQt5 Conexion DataBase/23.-Reporte Analisis de Datos 1.xlsx
@@ -576,13 +576,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="1" customWidth="1" min="1" max="1"/>
-    <col width="1.4" customWidth="1" min="2" max="2"/>
-    <col width="1.2" customWidth="1" min="3" max="3"/>
-    <col width="4.5" customWidth="1" min="4" max="4"/>
-    <col width="2" customWidth="1" min="5" max="5"/>
-    <col width="1" customWidth="1" min="6" max="6"/>
-    <col width="1" customWidth="1" min="7" max="7"/>
+    <col width="16.8" customWidth="1" min="1" max="1"/>
+    <col width="20.8" customWidth="1" min="2" max="2"/>
+    <col width="18.2" customWidth="1" min="3" max="3"/>
+    <col width="40" customWidth="1" min="4" max="4"/>
+    <col width="28.6" customWidth="1" min="5" max="5"/>
+    <col width="15.6" customWidth="1" min="6" max="6"/>
+    <col width="15.6" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
MechaBible Mark I: Programming - Python: Arduino GUI Multiple Windows, Database Connection, Data Analysis, Static Data Addition, Excell Cell Auto Adjustment & Excel Data Copy
</commit_message>
<xml_diff>
--- a/1.-Data Science/0.-Archivos_Ejercicios_Python/23.-GUI PyQt5 Conexion DataBase/23.-Reporte Analisis de Datos 1.xlsx
+++ b/1.-Data Science/0.-Archivos_Ejercicios_Python/23.-GUI PyQt5 Conexion DataBase/23.-Reporte Analisis de Datos 1.xlsx
@@ -581,7 +581,7 @@
     <col width="18.2" customWidth="1" min="3" max="3"/>
     <col width="40" customWidth="1" min="4" max="4"/>
     <col width="28.6" customWidth="1" min="5" max="5"/>
-    <col width="15.6" customWidth="1" min="6" max="6"/>
+    <col width="19.5" customWidth="1" min="6" max="6"/>
     <col width="15.6" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
@@ -743,6 +743,11 @@
           <t>Fecha de Publicacion</t>
         </is>
       </c>
+      <c r="F21" s="2" t="inlineStr">
+        <is>
+          <t>Static Column</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
@@ -770,6 +775,11 @@
           <t>10-01-2029</t>
         </is>
       </c>
+      <c r="F22" s="1" t="inlineStr">
+        <is>
+          <t>Static Text</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -797,6 +807,11 @@
           <t>05-04-2030</t>
         </is>
       </c>
+      <c r="F23" s="1" t="inlineStr">
+        <is>
+          <t>Static Text</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
@@ -824,6 +839,11 @@
           <t>23-05-2022</t>
         </is>
       </c>
+      <c r="F24" s="1" t="inlineStr">
+        <is>
+          <t>Static Text</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
@@ -851,6 +871,11 @@
           <t>10-10-2028</t>
         </is>
       </c>
+      <c r="F25" s="1" t="inlineStr">
+        <is>
+          <t>Static Text</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
@@ -878,6 +903,11 @@
           <t>09-09-2024</t>
         </is>
       </c>
+      <c r="F26" s="1" t="inlineStr">
+        <is>
+          <t>Static Text</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
@@ -903,6 +933,11 @@
       <c r="E27" s="1" t="inlineStr">
         <is>
           <t>01-12-2023</t>
+        </is>
+      </c>
+      <c r="F27" s="1" t="inlineStr">
+        <is>
+          <t>Static Text</t>
         </is>
       </c>
     </row>
@@ -1141,7 +1176,7 @@
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A21:E21">
+  <conditionalFormatting sqref="A21:F21">
     <cfRule type="notContainsBlanks" priority="19" dxfId="6">
       <formula>LEN(TRIM(A21))&gt;0</formula>
     </cfRule>
@@ -1160,7 +1195,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29:G29">
-    <cfRule type="notContainsBlanks" priority="31" dxfId="5">
+    <cfRule type="notContainsBlanks" priority="33" dxfId="5">
       <formula>LEN(TRIM(A29))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1170,12 +1205,6 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:G30">
-    <cfRule type="notContainsBlanks" priority="44" dxfId="12">
-      <formula>LEN(TRIM(A30))&gt;0</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" priority="45" dxfId="12">
-      <formula>LEN(TRIM(A30))&gt;0</formula>
-    </cfRule>
     <cfRule type="notContainsBlanks" priority="46" dxfId="12">
       <formula>LEN(TRIM(A30))&gt;0</formula>
     </cfRule>
@@ -1191,83 +1220,89 @@
     <cfRule type="notContainsBlanks" priority="50" dxfId="12">
       <formula>LEN(TRIM(A30))&gt;0</formula>
     </cfRule>
+    <cfRule type="notContainsBlanks" priority="51" dxfId="12">
+      <formula>LEN(TRIM(A30))&gt;0</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" priority="52" dxfId="12">
+      <formula>LEN(TRIM(A30))&gt;0</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31:G31">
-    <cfRule type="notContainsBlanks" priority="51" dxfId="13">
+    <cfRule type="notContainsBlanks" priority="53" dxfId="13">
       <formula>LEN(TRIM(A31))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
-    <cfRule type="notContainsBlanks" priority="64" dxfId="8">
+    <cfRule type="notContainsBlanks" priority="66" dxfId="8">
       <formula>LEN(TRIM(A32))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="65" dxfId="8">
+    <cfRule type="containsBlanks" priority="67" dxfId="8">
       <formula>LEN(TRIM(A32))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A33">
-    <cfRule type="notContainsBlanks" priority="78" dxfId="8">
+    <cfRule type="notContainsBlanks" priority="80" dxfId="8">
       <formula>LEN(TRIM(A33))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="79" dxfId="8">
+    <cfRule type="containsBlanks" priority="81" dxfId="8">
       <formula>LEN(TRIM(A33))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34">
-    <cfRule type="notContainsBlanks" priority="92" dxfId="8">
+    <cfRule type="notContainsBlanks" priority="94" dxfId="8">
       <formula>LEN(TRIM(A34))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="93" dxfId="8">
+    <cfRule type="containsBlanks" priority="95" dxfId="8">
       <formula>LEN(TRIM(A34))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35">
-    <cfRule type="notContainsBlanks" priority="106" dxfId="8">
+    <cfRule type="notContainsBlanks" priority="108" dxfId="8">
       <formula>LEN(TRIM(A35))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="107" dxfId="8">
+    <cfRule type="containsBlanks" priority="109" dxfId="8">
       <formula>LEN(TRIM(A35))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="notContainsBlanks" priority="120" dxfId="8">
+    <cfRule type="notContainsBlanks" priority="122" dxfId="8">
       <formula>LEN(TRIM(A36))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="121" dxfId="8">
+    <cfRule type="containsBlanks" priority="123" dxfId="8">
       <formula>LEN(TRIM(A36))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37">
-    <cfRule type="notContainsBlanks" priority="134" dxfId="8">
+    <cfRule type="notContainsBlanks" priority="136" dxfId="8">
       <formula>LEN(TRIM(A37))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="135" dxfId="8">
+    <cfRule type="containsBlanks" priority="137" dxfId="8">
       <formula>LEN(TRIM(A37))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38">
-    <cfRule type="notContainsBlanks" priority="148" dxfId="8">
+    <cfRule type="notContainsBlanks" priority="150" dxfId="8">
       <formula>LEN(TRIM(A38))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="149" dxfId="8">
+    <cfRule type="containsBlanks" priority="151" dxfId="8">
       <formula>LEN(TRIM(A38))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:G39">
-    <cfRule type="notContainsBlanks" priority="162" dxfId="13">
+    <cfRule type="notContainsBlanks" priority="164" dxfId="13">
       <formula>LEN(TRIM(A39))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40">
-    <cfRule type="notContainsBlanks" priority="175" dxfId="8">
+    <cfRule type="notContainsBlanks" priority="177" dxfId="8">
       <formula>LEN(TRIM(A40))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="176" dxfId="8">
+    <cfRule type="containsBlanks" priority="178" dxfId="8">
       <formula>LEN(TRIM(A40))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A41:G41">
-    <cfRule type="containsBlanks" priority="189" dxfId="2">
+    <cfRule type="containsBlanks" priority="191" dxfId="2">
       <formula>LEN(TRIM(A41))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1290,10 +1325,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="notContainsBlanks" priority="32" dxfId="9">
+    <cfRule type="notContainsBlanks" priority="34" dxfId="9">
       <formula>LEN(TRIM(B29))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="33" dxfId="9">
+    <cfRule type="containsBlanks" priority="35" dxfId="9">
       <formula>LEN(TRIM(B29))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1306,82 +1341,82 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="notContainsBlanks" priority="52" dxfId="9">
+    <cfRule type="notContainsBlanks" priority="54" dxfId="9">
       <formula>LEN(TRIM(B31))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="53" dxfId="9">
+    <cfRule type="containsBlanks" priority="55" dxfId="9">
       <formula>LEN(TRIM(B31))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="notContainsBlanks" priority="66" dxfId="9">
+    <cfRule type="notContainsBlanks" priority="68" dxfId="9">
       <formula>LEN(TRIM(B32))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="67" dxfId="9">
+    <cfRule type="containsBlanks" priority="69" dxfId="9">
       <formula>LEN(TRIM(B32))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33">
-    <cfRule type="notContainsBlanks" priority="80" dxfId="9">
+    <cfRule type="notContainsBlanks" priority="82" dxfId="9">
       <formula>LEN(TRIM(B33))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="81" dxfId="9">
+    <cfRule type="containsBlanks" priority="83" dxfId="9">
       <formula>LEN(TRIM(B33))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="notContainsBlanks" priority="94" dxfId="9">
+    <cfRule type="notContainsBlanks" priority="96" dxfId="9">
       <formula>LEN(TRIM(B34))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="95" dxfId="9">
+    <cfRule type="containsBlanks" priority="97" dxfId="9">
       <formula>LEN(TRIM(B34))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="notContainsBlanks" priority="108" dxfId="9">
+    <cfRule type="notContainsBlanks" priority="110" dxfId="9">
       <formula>LEN(TRIM(B35))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="109" dxfId="9">
+    <cfRule type="containsBlanks" priority="111" dxfId="9">
       <formula>LEN(TRIM(B35))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="notContainsBlanks" priority="122" dxfId="9">
+    <cfRule type="notContainsBlanks" priority="124" dxfId="9">
       <formula>LEN(TRIM(B36))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="123" dxfId="9">
+    <cfRule type="containsBlanks" priority="125" dxfId="9">
       <formula>LEN(TRIM(B36))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="notContainsBlanks" priority="136" dxfId="9">
+    <cfRule type="notContainsBlanks" priority="138" dxfId="9">
       <formula>LEN(TRIM(B37))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="137" dxfId="9">
+    <cfRule type="containsBlanks" priority="139" dxfId="9">
       <formula>LEN(TRIM(B37))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="notContainsBlanks" priority="150" dxfId="9">
+    <cfRule type="notContainsBlanks" priority="152" dxfId="9">
       <formula>LEN(TRIM(B38))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="151" dxfId="9">
+    <cfRule type="containsBlanks" priority="153" dxfId="9">
       <formula>LEN(TRIM(B38))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
-    <cfRule type="notContainsBlanks" priority="163" dxfId="9">
+    <cfRule type="notContainsBlanks" priority="165" dxfId="9">
       <formula>LEN(TRIM(B39))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="164" dxfId="9">
+    <cfRule type="containsBlanks" priority="166" dxfId="9">
       <formula>LEN(TRIM(B39))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40">
-    <cfRule type="notContainsBlanks" priority="177" dxfId="9">
+    <cfRule type="notContainsBlanks" priority="179" dxfId="9">
       <formula>LEN(TRIM(B40))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="178" dxfId="9">
+    <cfRule type="containsBlanks" priority="180" dxfId="9">
       <formula>LEN(TRIM(B40))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1394,10 +1429,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="notContainsBlanks" priority="34" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="36" dxfId="11">
       <formula>LEN(TRIM(C29))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="35" dxfId="11">
+    <cfRule type="containsBlanks" priority="37" dxfId="11">
       <formula>LEN(TRIM(C29))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1410,82 +1445,82 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="notContainsBlanks" priority="54" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="56" dxfId="11">
       <formula>LEN(TRIM(C31))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="55" dxfId="11">
+    <cfRule type="containsBlanks" priority="57" dxfId="11">
       <formula>LEN(TRIM(C31))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="notContainsBlanks" priority="68" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="70" dxfId="11">
       <formula>LEN(TRIM(C32))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="69" dxfId="11">
+    <cfRule type="containsBlanks" priority="71" dxfId="11">
       <formula>LEN(TRIM(C32))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="notContainsBlanks" priority="82" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="84" dxfId="11">
       <formula>LEN(TRIM(C33))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="83" dxfId="11">
+    <cfRule type="containsBlanks" priority="85" dxfId="11">
       <formula>LEN(TRIM(C33))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="notContainsBlanks" priority="96" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="98" dxfId="11">
       <formula>LEN(TRIM(C34))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="97" dxfId="11">
+    <cfRule type="containsBlanks" priority="99" dxfId="11">
       <formula>LEN(TRIM(C34))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="notContainsBlanks" priority="110" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="112" dxfId="11">
       <formula>LEN(TRIM(C35))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="111" dxfId="11">
+    <cfRule type="containsBlanks" priority="113" dxfId="11">
       <formula>LEN(TRIM(C35))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="notContainsBlanks" priority="124" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="126" dxfId="11">
       <formula>LEN(TRIM(C36))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="125" dxfId="11">
+    <cfRule type="containsBlanks" priority="127" dxfId="11">
       <formula>LEN(TRIM(C36))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="notContainsBlanks" priority="138" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="140" dxfId="11">
       <formula>LEN(TRIM(C37))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="139" dxfId="11">
+    <cfRule type="containsBlanks" priority="141" dxfId="11">
       <formula>LEN(TRIM(C37))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38">
-    <cfRule type="notContainsBlanks" priority="152" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="154" dxfId="11">
       <formula>LEN(TRIM(C38))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="153" dxfId="11">
+    <cfRule type="containsBlanks" priority="155" dxfId="11">
       <formula>LEN(TRIM(C38))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C39">
-    <cfRule type="notContainsBlanks" priority="165" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="167" dxfId="11">
       <formula>LEN(TRIM(C39))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="166" dxfId="11">
+    <cfRule type="containsBlanks" priority="168" dxfId="11">
       <formula>LEN(TRIM(C39))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="notContainsBlanks" priority="179" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="181" dxfId="11">
       <formula>LEN(TRIM(C40))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="180" dxfId="11">
+    <cfRule type="containsBlanks" priority="182" dxfId="11">
       <formula>LEN(TRIM(C40))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1498,90 +1533,90 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29">
-    <cfRule type="notContainsBlanks" priority="36" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="38" dxfId="11">
       <formula>LEN(TRIM(D29))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="37" dxfId="11">
+    <cfRule type="containsBlanks" priority="39" dxfId="11">
       <formula>LEN(TRIM(D29))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31">
-    <cfRule type="notContainsBlanks" priority="56" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="58" dxfId="11">
       <formula>LEN(TRIM(D31))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="57" dxfId="11">
+    <cfRule type="containsBlanks" priority="59" dxfId="11">
       <formula>LEN(TRIM(D31))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32">
-    <cfRule type="notContainsBlanks" priority="70" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="72" dxfId="11">
       <formula>LEN(TRIM(D32))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="71" dxfId="11">
+    <cfRule type="containsBlanks" priority="73" dxfId="11">
       <formula>LEN(TRIM(D32))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33">
-    <cfRule type="notContainsBlanks" priority="84" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="86" dxfId="11">
       <formula>LEN(TRIM(D33))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="85" dxfId="11">
+    <cfRule type="containsBlanks" priority="87" dxfId="11">
       <formula>LEN(TRIM(D33))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34">
-    <cfRule type="notContainsBlanks" priority="98" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="100" dxfId="11">
       <formula>LEN(TRIM(D34))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="99" dxfId="11">
+    <cfRule type="containsBlanks" priority="101" dxfId="11">
       <formula>LEN(TRIM(D34))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35">
-    <cfRule type="notContainsBlanks" priority="112" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="114" dxfId="11">
       <formula>LEN(TRIM(D35))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="113" dxfId="11">
+    <cfRule type="containsBlanks" priority="115" dxfId="11">
       <formula>LEN(TRIM(D35))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="notContainsBlanks" priority="126" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="128" dxfId="11">
       <formula>LEN(TRIM(D36))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="127" dxfId="11">
+    <cfRule type="containsBlanks" priority="129" dxfId="11">
       <formula>LEN(TRIM(D36))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37">
-    <cfRule type="notContainsBlanks" priority="140" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="142" dxfId="11">
       <formula>LEN(TRIM(D37))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="141" dxfId="11">
+    <cfRule type="containsBlanks" priority="143" dxfId="11">
       <formula>LEN(TRIM(D37))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D38">
-    <cfRule type="notContainsBlanks" priority="154" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="156" dxfId="11">
       <formula>LEN(TRIM(D38))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="155" dxfId="11">
+    <cfRule type="containsBlanks" priority="157" dxfId="11">
       <formula>LEN(TRIM(D38))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D39">
-    <cfRule type="notContainsBlanks" priority="167" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="169" dxfId="11">
       <formula>LEN(TRIM(D39))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="168" dxfId="11">
+    <cfRule type="containsBlanks" priority="170" dxfId="11">
       <formula>LEN(TRIM(D39))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D40">
-    <cfRule type="notContainsBlanks" priority="181" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="183" dxfId="11">
       <formula>LEN(TRIM(D40))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="182" dxfId="11">
+    <cfRule type="containsBlanks" priority="184" dxfId="11">
       <formula>LEN(TRIM(D40))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1594,266 +1629,274 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="notContainsBlanks" priority="38" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="40" dxfId="11">
       <formula>LEN(TRIM(E29))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="39" dxfId="11">
+    <cfRule type="containsBlanks" priority="41" dxfId="11">
       <formula>LEN(TRIM(E29))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="notContainsBlanks" priority="58" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="60" dxfId="11">
       <formula>LEN(TRIM(E31))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="59" dxfId="11">
+    <cfRule type="containsBlanks" priority="61" dxfId="11">
       <formula>LEN(TRIM(E31))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="notContainsBlanks" priority="72" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="74" dxfId="11">
       <formula>LEN(TRIM(E32))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="73" dxfId="11">
+    <cfRule type="containsBlanks" priority="75" dxfId="11">
       <formula>LEN(TRIM(E32))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33">
-    <cfRule type="notContainsBlanks" priority="86" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="88" dxfId="11">
       <formula>LEN(TRIM(E33))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="87" dxfId="11">
+    <cfRule type="containsBlanks" priority="89" dxfId="11">
       <formula>LEN(TRIM(E33))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="notContainsBlanks" priority="100" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="102" dxfId="11">
       <formula>LEN(TRIM(E34))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="101" dxfId="11">
+    <cfRule type="containsBlanks" priority="103" dxfId="11">
       <formula>LEN(TRIM(E34))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="notContainsBlanks" priority="114" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="116" dxfId="11">
       <formula>LEN(TRIM(E35))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="115" dxfId="11">
+    <cfRule type="containsBlanks" priority="117" dxfId="11">
       <formula>LEN(TRIM(E35))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36">
-    <cfRule type="notContainsBlanks" priority="128" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="130" dxfId="11">
       <formula>LEN(TRIM(E36))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="129" dxfId="11">
+    <cfRule type="containsBlanks" priority="131" dxfId="11">
       <formula>LEN(TRIM(E36))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37">
-    <cfRule type="notContainsBlanks" priority="142" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="144" dxfId="11">
       <formula>LEN(TRIM(E37))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="143" dxfId="11">
+    <cfRule type="containsBlanks" priority="145" dxfId="11">
       <formula>LEN(TRIM(E37))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38">
-    <cfRule type="notContainsBlanks" priority="156" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="158" dxfId="11">
       <formula>LEN(TRIM(E38))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="157" dxfId="11">
+    <cfRule type="containsBlanks" priority="159" dxfId="11">
       <formula>LEN(TRIM(E38))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39">
-    <cfRule type="notContainsBlanks" priority="169" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="171" dxfId="11">
       <formula>LEN(TRIM(E39))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="170" dxfId="11">
+    <cfRule type="containsBlanks" priority="172" dxfId="11">
       <formula>LEN(TRIM(E39))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="notContainsBlanks" priority="183" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="185" dxfId="11">
       <formula>LEN(TRIM(E40))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="184" dxfId="11">
+    <cfRule type="containsBlanks" priority="186" dxfId="11">
       <formula>LEN(TRIM(E40))=0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F22:F28">
+    <cfRule type="notContainsBlanks" priority="31" dxfId="10">
+      <formula>LEN(TRIM(F22))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" priority="32" dxfId="10">
+      <formula>LEN(TRIM(F22))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F29">
-    <cfRule type="notContainsBlanks" priority="40" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="42" dxfId="11">
       <formula>LEN(TRIM(F29))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="41" dxfId="11">
+    <cfRule type="containsBlanks" priority="43" dxfId="11">
       <formula>LEN(TRIM(F29))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F31">
-    <cfRule type="notContainsBlanks" priority="60" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="62" dxfId="11">
       <formula>LEN(TRIM(F31))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="61" dxfId="11">
+    <cfRule type="containsBlanks" priority="63" dxfId="11">
       <formula>LEN(TRIM(F31))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F32">
-    <cfRule type="notContainsBlanks" priority="74" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="76" dxfId="11">
       <formula>LEN(TRIM(F32))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="75" dxfId="11">
+    <cfRule type="containsBlanks" priority="77" dxfId="11">
       <formula>LEN(TRIM(F32))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F33">
-    <cfRule type="notContainsBlanks" priority="88" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="90" dxfId="11">
       <formula>LEN(TRIM(F33))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="89" dxfId="11">
+    <cfRule type="containsBlanks" priority="91" dxfId="11">
       <formula>LEN(TRIM(F33))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F34">
-    <cfRule type="notContainsBlanks" priority="102" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="104" dxfId="11">
       <formula>LEN(TRIM(F34))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="103" dxfId="11">
+    <cfRule type="containsBlanks" priority="105" dxfId="11">
       <formula>LEN(TRIM(F34))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F35">
-    <cfRule type="notContainsBlanks" priority="116" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="118" dxfId="11">
       <formula>LEN(TRIM(F35))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="117" dxfId="11">
+    <cfRule type="containsBlanks" priority="119" dxfId="11">
       <formula>LEN(TRIM(F35))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F36">
-    <cfRule type="notContainsBlanks" priority="130" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="132" dxfId="11">
       <formula>LEN(TRIM(F36))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="131" dxfId="11">
+    <cfRule type="containsBlanks" priority="133" dxfId="11">
       <formula>LEN(TRIM(F36))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F37">
-    <cfRule type="notContainsBlanks" priority="144" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="146" dxfId="11">
       <formula>LEN(TRIM(F37))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="145" dxfId="11">
+    <cfRule type="containsBlanks" priority="147" dxfId="11">
       <formula>LEN(TRIM(F37))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F38">
-    <cfRule type="notContainsBlanks" priority="158" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="160" dxfId="11">
       <formula>LEN(TRIM(F38))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="159" dxfId="11">
+    <cfRule type="containsBlanks" priority="161" dxfId="11">
       <formula>LEN(TRIM(F38))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F39">
-    <cfRule type="notContainsBlanks" priority="171" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="173" dxfId="11">
       <formula>LEN(TRIM(F39))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="172" dxfId="11">
+    <cfRule type="containsBlanks" priority="174" dxfId="11">
       <formula>LEN(TRIM(F39))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F40">
-    <cfRule type="notContainsBlanks" priority="185" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="187" dxfId="11">
       <formula>LEN(TRIM(F40))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="186" dxfId="11">
+    <cfRule type="containsBlanks" priority="188" dxfId="11">
       <formula>LEN(TRIM(F40))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G29">
-    <cfRule type="notContainsBlanks" priority="42" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="44" dxfId="11">
       <formula>LEN(TRIM(G29))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="43" dxfId="11">
+    <cfRule type="containsBlanks" priority="45" dxfId="11">
       <formula>LEN(TRIM(G29))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G31">
-    <cfRule type="notContainsBlanks" priority="62" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="64" dxfId="11">
       <formula>LEN(TRIM(G31))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="63" dxfId="11">
+    <cfRule type="containsBlanks" priority="65" dxfId="11">
       <formula>LEN(TRIM(G31))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32">
-    <cfRule type="notContainsBlanks" priority="76" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="78" dxfId="11">
       <formula>LEN(TRIM(G32))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="77" dxfId="11">
+    <cfRule type="containsBlanks" priority="79" dxfId="11">
       <formula>LEN(TRIM(G32))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33">
-    <cfRule type="notContainsBlanks" priority="90" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="92" dxfId="11">
       <formula>LEN(TRIM(G33))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="91" dxfId="11">
+    <cfRule type="containsBlanks" priority="93" dxfId="11">
       <formula>LEN(TRIM(G33))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34">
-    <cfRule type="notContainsBlanks" priority="104" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="106" dxfId="11">
       <formula>LEN(TRIM(G34))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="105" dxfId="11">
+    <cfRule type="containsBlanks" priority="107" dxfId="11">
       <formula>LEN(TRIM(G34))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G35">
-    <cfRule type="notContainsBlanks" priority="118" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="120" dxfId="11">
       <formula>LEN(TRIM(G35))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="119" dxfId="11">
+    <cfRule type="containsBlanks" priority="121" dxfId="11">
       <formula>LEN(TRIM(G35))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G36">
-    <cfRule type="notContainsBlanks" priority="132" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="134" dxfId="11">
       <formula>LEN(TRIM(G36))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="133" dxfId="11">
+    <cfRule type="containsBlanks" priority="135" dxfId="11">
       <formula>LEN(TRIM(G36))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G37">
-    <cfRule type="notContainsBlanks" priority="146" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="148" dxfId="11">
       <formula>LEN(TRIM(G37))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="147" dxfId="11">
+    <cfRule type="containsBlanks" priority="149" dxfId="11">
       <formula>LEN(TRIM(G37))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G38">
-    <cfRule type="notContainsBlanks" priority="160" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="162" dxfId="11">
       <formula>LEN(TRIM(G38))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="161" dxfId="11">
+    <cfRule type="containsBlanks" priority="163" dxfId="11">
       <formula>LEN(TRIM(G38))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G39">
-    <cfRule type="notContainsBlanks" priority="173" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="175" dxfId="11">
       <formula>LEN(TRIM(G39))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="174" dxfId="11">
+    <cfRule type="containsBlanks" priority="176" dxfId="11">
       <formula>LEN(TRIM(G39))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G40">
-    <cfRule type="notContainsBlanks" priority="187" dxfId="11">
+    <cfRule type="notContainsBlanks" priority="189" dxfId="11">
       <formula>LEN(TRIM(G40))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" priority="188" dxfId="11">
+    <cfRule type="containsBlanks" priority="190" dxfId="11">
       <formula>LEN(TRIM(G40))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>